<commit_message>
new code 11 added for plotting
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amirhosseindaraie/Desktop/project-code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3859B19-C5D3-F24C-8968-C4B83F5F1A1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6857D556-CA57-4147-8F9A-B8C44C7F51F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8100" yWindow="2340" windowWidth="18340" windowHeight="17440" xr2:uid="{DD1D188D-59F2-1C45-96A4-F38F60073F27}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="72">
   <si>
     <t>P18_N2 R</t>
   </si>
@@ -617,8 +617,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18BB5075-8B24-FF4F-86A9-B29637F3C505}">
   <dimension ref="A1:E61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="200" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" zoomScale="200" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -754,6 +754,9 @@
       <c r="A12" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="B12" s="1" t="s">
+        <v>71</v>
+      </c>
       <c r="D12" s="1" t="s">
         <v>16</v>
       </c>
@@ -765,6 +768,9 @@
       <c r="A13" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="B13" s="1" t="s">
+        <v>71</v>
+      </c>
       <c r="D13" s="1" t="s">
         <v>17</v>
       </c>
@@ -776,6 +782,9 @@
       <c r="A14" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="B14" s="1" t="s">
+        <v>71</v>
+      </c>
       <c r="D14" s="1" t="s">
         <v>18</v>
       </c>
@@ -787,11 +796,17 @@
       <c r="A15" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="B15" s="1" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>25</v>
       </c>
+      <c r="B16" s="1" t="s">
+        <v>71</v>
+      </c>
       <c r="D16" s="1">
         <f>SUBTOTAL(3,D7:D14)</f>
         <v>8</v>
@@ -801,229 +816,364 @@
         <v>61</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B17" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B18" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B19" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B20" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B21" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B22" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B23" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B24" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B25" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B26" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B27" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B28" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B29" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B30" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B31" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B32" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B33" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B34" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B35" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B36" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B37" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B38" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B39" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B40" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B41" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B42" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B43" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B44" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B45" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B46" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B47" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B48" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B49" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B50" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B51" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B52" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B53" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B54" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B55" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B56" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B57" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B58" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B59" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B60" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>70</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
last code for 21
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amirhosseindaraie/Desktop/project-code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D631E56A-7198-D943-B5B0-FD23B7C93437}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09FBD3F6-52FF-7447-9341-91973D65CAB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8100" yWindow="2340" windowWidth="18340" windowHeight="17440" xr2:uid="{DD1D188D-59F2-1C45-96A4-F38F60073F27}"/>
   </bookViews>
@@ -258,7 +258,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="[$-3000401]0.##"/>
+    <numFmt numFmtId="164" formatCode="[$-3000401]0.##"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -337,11 +337,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
   </cellXfs>

</xml_diff>